<commit_message>
Update the documentation with for 'Tabella comuni subentrati'
</commit_message>
<xml_diff>
--- a/src/_static/xlsx/tab_Stato_validazione_del_codice_fiscale.xlsx
+++ b/src/_static/xlsx/tab_Stato_validazione_del_codice_fiscale.xlsx
@@ -7,15 +7,14 @@
     <workbookView xWindow="630" yWindow="615" windowWidth="20700" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="SQL Results" sheetId="1" r:id="rId1"/>
-    <sheet name="SQL Statement" sheetId="2" r:id="rId2"/>
+    <sheet name="Codici validazione CF" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>ID</t>
   </si>
@@ -23,46 +22,16 @@
     <t>DESCRIZIONE</t>
   </si>
   <si>
-    <t>ORDINAMENTO</t>
+    <t>Dati anagrafici non validati ( soggetto non presente in Agenzia Entrate o iscritto senza validazione )</t>
   </si>
   <si>
-    <t>DATAINIZIOVALIDITA</t>
-  </si>
-  <si>
-    <t>DATAFINEVALIDITA</t>
-  </si>
-  <si>
-    <t>Dati anagrafici validati ( soggetto presente in A.T. con  dati anagrafici uguali a quelli indicati dal Comune ma CF diverso)</t>
-  </si>
-  <si>
-    <t>01/01/1900</t>
-  </si>
-  <si>
-    <t>Dati anagrafici diversi (soggetto presente in A.T. con  dati anagrafici diversi da quelli indicati dal Comune; la differenza non produce un diverso codice fiscale)</t>
-  </si>
-  <si>
-    <t>Posizione con  codice fiscale collegato  (più recente) (soggetto presente in A.T., individuato con il codice fiscale collegato)</t>
-  </si>
-  <si>
-    <t>Posizione con  più omocodici collegati  (soggetto presente in A.T., ma non individuato con il codice fiscale omocodice)</t>
-  </si>
-  <si>
-    <t>Posizione inesistente (soggetto NON presente in A.T.)</t>
-  </si>
-  <si>
-    <t>Dati anagrafici validati ( soggetto presente in A.T. con  CF e dati anagrafici uguali a quelli indicati dal Comune)</t>
-  </si>
-  <si>
-    <t>select * from DEC_STATO_CF t</t>
+    <t>Dati anagrafici validati ( soggetto presente in Agenzia Entrate. con  CF e dati anagrafici uguali a quelli indicati dal Comune)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd\/mm\/yyyy"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
@@ -100,9 +69,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -405,121 +373,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.1640625"/>
     <col min="2" max="2" width="50"/>
-    <col min="3" max="3" width="13.6640625"/>
-    <col min="4" max="4" width="17.1640625"/>
-    <col min="5" max="5" width="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1">
-        <v>2958465</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2958465</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2958465</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1">
-        <v>2958465</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1">
-        <v>2958465</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="1">
-        <v>2958465</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -530,23 +418,170 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="80"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0EB43895666D743BBE5EE80DE8AFF2D" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3898ec998cc85d3bcc261598fbbf3dc9">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all/>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8899EA95-DE9D-4AA3-972C-67E89342E423}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69831F9B-A01C-47DE-88F1-3A0785CA53A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EBE875E-8464-4351-B0DA-AC819C4DA4D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>